<commit_message>
Updated to Ninject 3.0.0.15 and Petite 0.3.2
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="21315" windowHeight="10035"/>
@@ -72,8 +72,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,43 +130,20 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="107"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="7"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="7"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>(Tabelle1!$A$2:$A$12,Tabelle1!$A$14:$A$17)</c:f>
@@ -275,57 +252,41 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="cylinder"/>
-        <c:axId val="191414656"/>
-        <c:axId val="191416192"/>
+        <c:axId val="88904448"/>
+        <c:axId val="88905984"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="191414656"/>
+        <c:axId val="88904448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191416192"/>
+        <c:crossAx val="88905984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191416192"/>
+        <c:axId val="88905984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191414656"/>
+        <c:crossAx val="88904448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -337,43 +298,20 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="107"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="7"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="7"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>(Tabelle1!$A$2:$A$12,Tabelle1!$A$14:$A$17)</c:f>
@@ -482,57 +420,41 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="cylinder"/>
-        <c:axId val="193349120"/>
-        <c:axId val="193350656"/>
+        <c:axId val="146220928"/>
+        <c:axId val="146222464"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="193349120"/>
+        <c:axId val="146220928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193350656"/>
+        <c:crossAx val="146222464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193350656"/>
+        <c:axId val="146222464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193349120"/>
+        <c:crossAx val="146220928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -544,43 +466,20 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="107"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="7"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="7"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>(Tabelle1!$A$2:$A$12,Tabelle1!$A$14:$A$17)</c:f>
@@ -689,57 +588,41 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="cylinder"/>
-        <c:axId val="193358464"/>
-        <c:axId val="193380736"/>
+        <c:axId val="146246656"/>
+        <c:axId val="146252544"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="193358464"/>
+        <c:axId val="146246656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193380736"/>
+        <c:crossAx val="146252544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193380736"/>
+        <c:axId val="146252544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193358464"/>
+        <c:crossAx val="146246656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -845,7 +728,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -919,7 +802,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -954,7 +836,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1130,19 +1011,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1156,7 +1037,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1170,7 +1051,7 @@
         <v>6485</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1184,7 +1065,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1198,7 +1079,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1212,7 +1093,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1226,7 +1107,7 @@
         <v>2787</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1121,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1254,7 +1135,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1268,7 +1149,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1163,7 @@
         <v>35821</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1296,7 +1177,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1310,7 +1191,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1205,7 @@
         <v>67208</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1219,7 @@
         <v>4517</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1352,7 +1233,7 @@
         <v>8852</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1366,7 +1247,7 @@
         <v>4911</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1388,24 +1269,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support for Managed Extensibility Framework (MEF)
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">AutoFac       </t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Mugen</t>
+  </si>
+  <si>
+    <t>MEF</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -150,9 +155,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$13,Tabelle1!$A$15:$A$18)</c:f>
+              <c:f>(Tabelle1!$A$2:$A$14,Tabelle1!$A$16:$A$19)</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>AutoFac       </c:v>
                 </c:pt>
@@ -175,30 +180,33 @@
                   <c:v>LinFu         </c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>MEF</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Mugen</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Munq          </c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Ninject       </c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Petite        </c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>SimpleInjector</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>StructureMap  </c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>TinyIOC       </c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Unity         </c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Windsor       </c:v>
                 </c:pt>
               </c:strCache>
@@ -206,10 +214,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$B$2:$B$13,Tabelle1!$B$15:$B$18)</c:f>
+              <c:f>(Tabelle1!$B$2:$B$14,Tabelle1!$B$16:$B$19)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>711</c:v>
                 </c:pt>
@@ -232,30 +240,33 @@
                   <c:v>2738</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>2838</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>390</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>99</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>5148</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1142</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>423</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>869</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>633</c:v>
                 </c:pt>
               </c:numCache>
@@ -263,25 +274,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="132689920"/>
-        <c:axId val="132691456"/>
+        <c:axId val="135357952"/>
+        <c:axId val="135359488"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="132689920"/>
+        <c:axId val="135357952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132691456"/>
+        <c:crossAx val="135359488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132691456"/>
+        <c:axId val="135359488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,7 +300,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132689920"/>
+        <c:crossAx val="135357952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -323,9 +334,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$13,Tabelle1!$A$15:$A$18)</c:f>
+              <c:f>(Tabelle1!$A$2:$A$14,Tabelle1!$A$16:$A$19)</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>AutoFac       </c:v>
                 </c:pt>
@@ -348,30 +359,33 @@
                   <c:v>LinFu         </c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>MEF</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Mugen</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Munq          </c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Ninject       </c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Petite        </c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>SimpleInjector</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>StructureMap  </c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>TinyIOC       </c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Unity         </c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Windsor       </c:v>
                 </c:pt>
               </c:strCache>
@@ -379,10 +393,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$C$2:$C$13,Tabelle1!$C$15:$C$18)</c:f>
+              <c:f>(Tabelle1!$C$2:$C$14,Tabelle1!$C$16:$C$19)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>2423</c:v>
                 </c:pt>
@@ -405,30 +419,33 @@
                   <c:v>15542</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>9931</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>754</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>15084</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>105</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1185</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>2072</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1283</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>2029</c:v>
                 </c:pt>
               </c:numCache>
@@ -436,25 +453,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="132723456"/>
-        <c:axId val="132724992"/>
+        <c:axId val="135809280"/>
+        <c:axId val="135811072"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="132723456"/>
+        <c:axId val="135809280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132724992"/>
+        <c:crossAx val="135811072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132724992"/>
+        <c:axId val="135811072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,7 +479,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132723456"/>
+        <c:crossAx val="135809280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -496,9 +513,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$13,Tabelle1!$A$15:$A$18)</c:f>
+              <c:f>(Tabelle1!$A$2:$A$14,Tabelle1!$A$16:$A$19)</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>AutoFac       </c:v>
                 </c:pt>
@@ -521,30 +538,33 @@
                   <c:v>LinFu         </c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>MEF</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Mugen</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Munq          </c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Ninject       </c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Petite        </c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>SimpleInjector</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>StructureMap  </c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>TinyIOC       </c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Unity         </c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Windsor       </c:v>
                 </c:pt>
               </c:strCache>
@@ -552,10 +572,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$D$2:$D$13,Tabelle1!$D$15:$D$18)</c:f>
+              <c:f>(Tabelle1!$D$2:$D$14,Tabelle1!$D$16:$D$19)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>6077</c:v>
                 </c:pt>
@@ -578,30 +598,33 @@
                   <c:v>41080</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>27133</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2237</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>382</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>39241</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>118</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>4001</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>8416</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>4466</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>6313</c:v>
                 </c:pt>
               </c:numCache>
@@ -609,25 +632,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="132744704"/>
-        <c:axId val="132746240"/>
+        <c:axId val="135822336"/>
+        <c:axId val="135836416"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="132744704"/>
+        <c:axId val="135822336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132746240"/>
+        <c:crossAx val="135836416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132746240"/>
+        <c:axId val="135836416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +658,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132744704"/>
+        <c:crossAx val="135822336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -657,13 +680,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>8620</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -687,13 +710,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -717,13 +740,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1031,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1043,7 +1066,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B1">
@@ -1057,7 +1080,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -1071,7 +1094,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -1085,7 +1108,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -1099,7 +1122,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2">
@@ -1113,7 +1136,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2">
@@ -1127,7 +1150,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2">
@@ -1141,7 +1164,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2">
@@ -1156,141 +1179,155 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2838</v>
+      </c>
+      <c r="C9" s="2">
+        <v>9931</v>
+      </c>
+      <c r="D9" s="2">
+        <v>27133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>390</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>754</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>2237</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>99</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>124</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>382</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
         <v>5148</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="2">
         <v>15084</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>39241</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>91</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>91</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>80</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>105</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>31574</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>43197</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>63920</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>1142</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>1185</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>4001</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>423</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>2072</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>8416</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>869</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>1283</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>4466</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>633</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>2029</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>6313</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Ninject, Autofac, MunqS, SimpleInjector and Griffin
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -225,7 +225,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>711</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>71</c:v>
@@ -234,7 +234,7 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>313</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>116</c:v>
@@ -258,13 +258,13 @@
                   <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5148</c:v>
+                  <c:v>5792</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>80</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1142</c:v>
@@ -283,25 +283,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="99587584"/>
-        <c:axId val="99589120"/>
+        <c:axId val="140576256"/>
+        <c:axId val="140577792"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="99587584"/>
+        <c:axId val="140576256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99589120"/>
+        <c:crossAx val="140577792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99589120"/>
+        <c:axId val="140577792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -309,7 +309,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99587584"/>
+        <c:crossAx val="140576256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -410,7 +410,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2423</c:v>
+                  <c:v>1946</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>72</c:v>
@@ -419,7 +419,7 @@
                   <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>334</c:v>
+                  <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>115</c:v>
@@ -443,13 +443,13 @@
                   <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15084</c:v>
+                  <c:v>16201</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>105</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1185</c:v>
@@ -468,25 +468,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="99952896"/>
-        <c:axId val="99954688"/>
+        <c:axId val="140626176"/>
+        <c:axId val="140627968"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="99952896"/>
+        <c:axId val="140626176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99954688"/>
+        <c:crossAx val="140627968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="l"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99954688"/>
+        <c:axId val="140627968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +494,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99952896"/>
+        <c:crossAx val="140626176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -595,7 +595,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>6077</c:v>
+                  <c:v>4941</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>125</c:v>
@@ -604,7 +604,7 @@
                   <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>767</c:v>
+                  <c:v>485</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>129</c:v>
@@ -628,13 +628,13 @@
                   <c:v>382</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>39241</c:v>
+                  <c:v>44863</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>118</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>4001</c:v>
@@ -653,25 +653,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="99965952"/>
-        <c:axId val="99984128"/>
+        <c:axId val="140639232"/>
+        <c:axId val="140665600"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="99965952"/>
+        <c:axId val="140639232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99984128"/>
+        <c:crossAx val="140665600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99984128"/>
+        <c:axId val="140665600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +679,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99965952"/>
+        <c:crossAx val="140639232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1077,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1105,13 +1105,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>711</v>
+        <v>660</v>
       </c>
       <c r="C2">
-        <v>2423</v>
+        <v>1946</v>
       </c>
       <c r="D2">
-        <v>6077</v>
+        <v>4941</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1147,13 +1147,13 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>313</v>
+        <v>184</v>
       </c>
       <c r="C5">
-        <v>334</v>
+        <v>181</v>
       </c>
       <c r="D5">
-        <v>767</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1259,13 +1259,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="2">
-        <v>5148</v>
+        <v>5792</v>
       </c>
       <c r="C13" s="2">
-        <v>15084</v>
+        <v>16201</v>
       </c>
       <c r="D13" s="2">
-        <v>39241</v>
+        <v>44863</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1287,13 +1287,13 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D15">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:4">

</xml_diff>

<commit_message>
Updated IoCs: Castle Windsor 3.1.0 Unity 2.1.505.2 structuremap 2.6.4.1 Simple Injector 1.5.0.12199 LightInject 2.0.0.0 MugenInjection 2.6.0
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -121,11 +121,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -222,94 +222,94 @@
             <c:numRef>
               <c:f>(Tabelle1!$B$2:$B$15,Tabelle1!$B$17:$B$20)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>660</c:v>
+                  <c:v>715</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>184</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>116</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>158</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>104</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2738</c:v>
+                  <c:v>3053</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2838</c:v>
+                  <c:v>3211</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>390</c:v>
+                  <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>99</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5792</c:v>
+                  <c:v>5785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>79</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1142</c:v>
+                  <c:v>1161</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>423</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>869</c:v>
+                  <c:v>898</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>633</c:v>
+                  <c:v>372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="140576256"/>
-        <c:axId val="140577792"/>
+        <c:axId val="107927040"/>
+        <c:axId val="107928576"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="140576256"/>
+        <c:axId val="107927040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140577792"/>
+        <c:crossAx val="107928576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140577792"/>
+        <c:axId val="107928576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140576256"/>
+        <c:crossAx val="107927040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -407,94 +407,94 @@
             <c:numRef>
               <c:f>(Tabelle1!$C$2:$C$15,Tabelle1!$C$17:$C$20)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1946</c:v>
+                  <c:v>1896</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>181</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>115</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>535</c:v>
+                  <c:v>584</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>106</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15542</c:v>
+                  <c:v>17167</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9931</c:v>
+                  <c:v>10230</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>754</c:v>
+                  <c:v>585</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>124</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16201</c:v>
+                  <c:v>16188</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1185</c:v>
+                  <c:v>1244</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2072</c:v>
+                  <c:v>1964</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1283</c:v>
+                  <c:v>1386</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2029</c:v>
+                  <c:v>1677</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="140626176"/>
-        <c:axId val="140627968"/>
+        <c:axId val="108292352"/>
+        <c:axId val="108294144"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="140626176"/>
+        <c:axId val="108292352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140627968"/>
+        <c:crossAx val="108294144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="l"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140627968"/>
+        <c:axId val="108294144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140626176"/>
+        <c:crossAx val="108292352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -592,94 +592,94 @@
             <c:numRef>
               <c:f>(Tabelle1!$D$2:$D$15,Tabelle1!$D$17:$D$20)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>4941</c:v>
+                  <c:v>5069</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>265</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>485</c:v>
+                  <c:v>474</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>129</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2761</c:v>
+                  <c:v>3031</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>114</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41080</c:v>
+                  <c:v>45440</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27133</c:v>
+                  <c:v>27582</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2237</c:v>
+                  <c:v>2081</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>382</c:v>
+                  <c:v>392</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44863</c:v>
+                  <c:v>46694</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>270</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>113</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4001</c:v>
+                  <c:v>4237</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8416</c:v>
+                  <c:v>7665</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4466</c:v>
+                  <c:v>4874</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6313</c:v>
+                  <c:v>5402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="140639232"/>
-        <c:axId val="140665600"/>
+        <c:axId val="108305408"/>
+        <c:axId val="108319488"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="140639232"/>
+        <c:axId val="108305408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140665600"/>
+        <c:crossAx val="108319488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140665600"/>
+        <c:axId val="108319488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140639232"/>
+        <c:crossAx val="108305408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1075,296 +1075,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1">
-        <v>39</v>
-      </c>
-      <c r="C1">
-        <v>41</v>
-      </c>
-      <c r="D1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="2">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>660</v>
-      </c>
-      <c r="C2">
-        <v>1946</v>
-      </c>
-      <c r="D2">
-        <v>4941</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="2">
+        <v>715</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1896</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5069</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>71</v>
-      </c>
-      <c r="C3" s="1">
-        <v>72</v>
-      </c>
-      <c r="D3" s="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="2">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2">
+        <v>87</v>
+      </c>
+      <c r="D3" s="2">
+        <v>131</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>97</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="2">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2">
+        <v>260</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>189</v>
+      </c>
+      <c r="C5" s="2">
+        <v>186</v>
+      </c>
+      <c r="D5" s="2">
+        <v>474</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
         <v>109</v>
       </c>
-      <c r="D4">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>184</v>
-      </c>
-      <c r="C5">
-        <v>181</v>
-      </c>
-      <c r="D5">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2">
-        <v>116</v>
-      </c>
       <c r="C6" s="2">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D6" s="2">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C7" s="2">
-        <v>535</v>
+        <v>584</v>
       </c>
       <c r="D7" s="2">
-        <v>2761</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
+        <v>3031</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>104</v>
-      </c>
-      <c r="C8" s="2">
-        <v>106</v>
-      </c>
-      <c r="D8" s="2">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="3">
+        <v>84</v>
+      </c>
+      <c r="D8" s="3">
+        <v>96</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2">
-        <v>2738</v>
+        <v>3053</v>
       </c>
       <c r="C9" s="2">
-        <v>15542</v>
+        <v>17167</v>
       </c>
       <c r="D9" s="2">
-        <v>41080</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
+        <v>45440</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2">
-        <v>2838</v>
+        <v>3211</v>
       </c>
       <c r="C10" s="2">
-        <v>9931</v>
+        <v>10230</v>
       </c>
       <c r="D10" s="2">
-        <v>27133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+        <v>27582</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>390</v>
+        <v>341</v>
       </c>
       <c r="C11" s="2">
-        <v>754</v>
+        <v>585</v>
       </c>
       <c r="D11" s="2">
-        <v>2237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
+        <v>2081</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C12" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D12" s="2">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="2">
-        <v>5792</v>
+        <v>5785</v>
       </c>
       <c r="C13" s="2">
-        <v>16201</v>
+        <v>16188</v>
       </c>
       <c r="D13" s="2">
-        <v>44863</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
+        <v>46694</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
-        <v>91</v>
-      </c>
-      <c r="C14">
-        <v>91</v>
-      </c>
-      <c r="D14">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="2">
+        <v>93</v>
+      </c>
+      <c r="C14" s="2">
+        <v>90</v>
+      </c>
+      <c r="D14" s="2">
+        <v>272</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15">
-        <v>79</v>
-      </c>
-      <c r="C15">
-        <v>96</v>
-      </c>
-      <c r="D15">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="3">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2">
+        <v>102</v>
+      </c>
+      <c r="D15" s="2">
+        <v>144</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16">
-        <v>31574</v>
-      </c>
-      <c r="C16">
-        <v>43197</v>
-      </c>
-      <c r="D16">
-        <v>63920</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+      <c r="B16" s="2">
+        <v>32629</v>
+      </c>
+      <c r="C16" s="2">
+        <v>46622</v>
+      </c>
+      <c r="D16" s="2">
+        <v>65291</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17">
-        <v>1142</v>
-      </c>
-      <c r="C17">
-        <v>1185</v>
-      </c>
-      <c r="D17">
-        <v>4001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
+      <c r="B17" s="2">
+        <v>1161</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1244</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4237</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>423</v>
-      </c>
-      <c r="C18">
-        <v>2072</v>
-      </c>
-      <c r="D18">
-        <v>8416</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
+      <c r="B18" s="2">
+        <v>424</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1964</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7665</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19">
-        <v>869</v>
-      </c>
-      <c r="C19">
-        <v>1283</v>
-      </c>
-      <c r="D19">
-        <v>4466</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
+      <c r="B19" s="2">
+        <v>898</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1386</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4874</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20">
-        <v>633</v>
-      </c>
-      <c r="C20">
-        <v>2029</v>
-      </c>
-      <c r="D20">
-        <v>6313</v>
-      </c>
+      <c r="B20" s="2">
+        <v>372</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1677</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5402</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Griffin and LightInject.
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -243,7 +243,7 @@
                   <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3053</c:v>
@@ -283,25 +283,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="107927040"/>
-        <c:axId val="107928576"/>
+        <c:axId val="141540352"/>
+        <c:axId val="77050624"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="107927040"/>
+        <c:axId val="141540352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107928576"/>
+        <c:crossAx val="77050624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107928576"/>
+        <c:axId val="77050624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -309,7 +309,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107927040"/>
+        <c:crossAx val="141540352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -428,7 +428,7 @@
                   <c:v>584</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>84</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17167</c:v>
@@ -468,25 +468,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="108292352"/>
-        <c:axId val="108294144"/>
+        <c:axId val="77082624"/>
+        <c:axId val="77084160"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="108292352"/>
+        <c:axId val="77082624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108294144"/>
+        <c:crossAx val="77084160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="l"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108294144"/>
+        <c:axId val="77084160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +494,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108292352"/>
+        <c:crossAx val="77082624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -613,7 +613,7 @@
                   <c:v>3031</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>45440</c:v>
@@ -653,25 +653,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="108305408"/>
-        <c:axId val="108319488"/>
+        <c:axId val="77124352"/>
+        <c:axId val="77125888"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="108305408"/>
+        <c:axId val="77124352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108319488"/>
+        <c:crossAx val="77125888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108319488"/>
+        <c:axId val="77125888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +679,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108305408"/>
+        <c:crossAx val="77124352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1077,7 +1077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -1205,13 +1207,13 @@
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C8" s="3">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>

</xml_diff>

<commit_message>
-Updated MugenInjection (2.6.0 -> 3.0.0) -Updated Dynamo (1.0 -> 3.0.1.0)
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -122,13 +122,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -231,86 +232,86 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>715</c:v>
+                  <c:v>664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>139</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>189</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>165</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3053</c:v>
+                  <c:v>2924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3211</c:v>
+                  <c:v>2698</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>341</c:v>
+                  <c:v>434</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>101</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5785</c:v>
+                  <c:v>7385</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>93</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1161</c:v>
+                  <c:v>1136</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>424</c:v>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>898</c:v>
+                  <c:v>1153</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>372</c:v>
+                  <c:v>485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="152423424"/>
-        <c:axId val="155665152"/>
+        <c:axId val="140274688"/>
+        <c:axId val="82039552"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="152423424"/>
+        <c:axId val="140274688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155665152"/>
+        <c:crossAx val="82039552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155665152"/>
+        <c:axId val="82039552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -318,7 +319,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152423424"/>
+        <c:crossAx val="140274688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -422,86 +423,86 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>1896</c:v>
+                  <c:v>2093</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37387</c:v>
+                  <c:v>31564</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>102</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>186</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>110</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>584</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17167</c:v>
+                  <c:v>17448</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10230</c:v>
+                  <c:v>9994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>585</c:v>
+                  <c:v>693</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>122</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16188</c:v>
+                  <c:v>19487</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1244</c:v>
+                  <c:v>1187</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1964</c:v>
+                  <c:v>2175</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1386</c:v>
+                  <c:v>1872</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1677</c:v>
+                  <c:v>2505</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="155705344"/>
-        <c:axId val="155706880"/>
+        <c:axId val="82083840"/>
+        <c:axId val="82085376"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="155705344"/>
+        <c:axId val="82083840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155706880"/>
+        <c:crossAx val="82085376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="l"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155706880"/>
+        <c:axId val="82085376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +510,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155705344"/>
+        <c:crossAx val="82083840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -613,86 +614,86 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5069</c:v>
+                  <c:v>5174</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77129</c:v>
+                  <c:v>69224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>131</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>474</c:v>
+                  <c:v>458</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2796</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47403</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28197</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1599</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54468</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>117</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>3031</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45440</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>27582</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2081</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>392</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>46694</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>272</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>103</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>4237</c:v>
+                  <c:v>4407</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7665</c:v>
+                  <c:v>7289</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4874</c:v>
+                  <c:v>6202</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5402</c:v>
+                  <c:v>7012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="156254976"/>
-        <c:axId val="156256512"/>
+        <c:axId val="82113280"/>
+        <c:axId val="82114816"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="156254976"/>
+        <c:axId val="82113280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156256512"/>
+        <c:crossAx val="82114816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156256512"/>
+        <c:axId val="82114816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,7 +701,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156254976"/>
+        <c:crossAx val="82113280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1099,7 +1100,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B16" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1126,13 +1127,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>715</v>
+        <v>664</v>
       </c>
       <c r="C2" s="2">
-        <v>1896</v>
+        <v>2093</v>
       </c>
       <c r="D2" s="2">
-        <v>5069</v>
+        <v>5174</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1143,13 +1144,13 @@
         <v>20</v>
       </c>
       <c r="B3" s="2">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C3" s="2">
-        <v>37387</v>
+        <v>31564</v>
       </c>
       <c r="D3" s="2">
-        <v>77129</v>
+        <v>69224</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1162,11 +1163,11 @@
       <c r="B4" s="2">
         <v>74</v>
       </c>
-      <c r="C4" s="2">
-        <v>87</v>
+      <c r="C4" s="3">
+        <v>79</v>
       </c>
       <c r="D4" s="2">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1177,13 +1178,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1194,13 +1195,13 @@
         <v>19</v>
       </c>
       <c r="B6" s="2">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C6" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="2">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1211,13 +1212,13 @@
         <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1228,13 +1229,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C8" s="2">
-        <v>584</v>
+        <v>472</v>
       </c>
       <c r="D8" s="2">
-        <v>3031</v>
+        <v>2796</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1245,13 +1246,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>74</v>
-      </c>
-      <c r="C9" s="3">
-        <v>78</v>
+        <v>117</v>
+      </c>
+      <c r="C9" s="4">
+        <v>84</v>
       </c>
       <c r="D9" s="3">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1262,13 +1263,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>3053</v>
+        <v>2924</v>
       </c>
       <c r="C10" s="2">
-        <v>17167</v>
+        <v>17448</v>
       </c>
       <c r="D10" s="2">
-        <v>45440</v>
+        <v>47403</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1279,13 +1280,13 @@
         <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>3211</v>
+        <v>2698</v>
       </c>
       <c r="C11" s="2">
-        <v>10230</v>
+        <v>9994</v>
       </c>
       <c r="D11" s="2">
-        <v>27582</v>
+        <v>28197</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1296,13 +1297,13 @@
         <v>17</v>
       </c>
       <c r="B12" s="2">
-        <v>341</v>
+        <v>434</v>
       </c>
       <c r="C12" s="2">
-        <v>585</v>
+        <v>693</v>
       </c>
       <c r="D12" s="2">
-        <v>2081</v>
+        <v>1599</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1313,13 +1314,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C13" s="2">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D13" s="2">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1330,13 +1331,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="2">
-        <v>5785</v>
+        <v>7385</v>
       </c>
       <c r="C14" s="2">
-        <v>16188</v>
+        <v>19487</v>
       </c>
       <c r="D14" s="2">
-        <v>46694</v>
+        <v>54468</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1347,13 +1348,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="2">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C15" s="2">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1367,10 +1368,10 @@
         <v>70</v>
       </c>
       <c r="C16" s="2">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D16" s="2">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1381,13 +1382,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="2">
-        <v>32629</v>
+        <v>811</v>
       </c>
       <c r="C17" s="2">
-        <v>46622</v>
+        <v>13566</v>
       </c>
       <c r="D17" s="2">
-        <v>65291</v>
+        <v>37640</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1398,13 +1399,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="2">
-        <v>1161</v>
+        <v>1136</v>
       </c>
       <c r="C18" s="2">
-        <v>1244</v>
+        <v>1187</v>
       </c>
       <c r="D18" s="2">
-        <v>4237</v>
+        <v>4407</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1415,13 +1416,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="2">
-        <v>424</v>
+        <v>466</v>
       </c>
       <c r="C19" s="2">
-        <v>1964</v>
+        <v>2175</v>
       </c>
       <c r="D19" s="2">
-        <v>7665</v>
+        <v>7289</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1432,13 +1433,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="2">
-        <v>898</v>
+        <v>1153</v>
       </c>
       <c r="C20" s="2">
-        <v>1386</v>
+        <v>1872</v>
       </c>
       <c r="D20" s="2">
-        <v>4874</v>
+        <v>6202</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1449,13 +1450,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="2">
-        <v>372</v>
+        <v>485</v>
       </c>
       <c r="C21" s="2">
-        <v>1677</v>
+        <v>2505</v>
       </c>
       <c r="D21" s="2">
-        <v>5402</v>
+        <v>7012</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>

</xml_diff>

<commit_message>
Updated to Catel 3.4, Griffin.Container 1.1.0, SimpleInjector 1.6.0.12319, TinyIoC 1.2
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -162,9 +162,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$16,Tabelle1!$A$18:$A$21)</c:f>
+              <c:f>Tabelle1!$A$2:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>AutoFac       </c:v>
                 </c:pt>
@@ -211,15 +211,18 @@
                   <c:v>SimpleInjector</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>Spring.NET    </c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>StructureMap  </c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>TinyIOC       </c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Unity         </c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Windsor       </c:v>
                 </c:pt>
               </c:strCache>
@@ -227,91 +230,94 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$B$2:$B$16,Tabelle1!$B$18:$B$21)</c:f>
+              <c:f>Tabelle1!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>664</c:v>
+                  <c:v>658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>176</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>162</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>117</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2924</c:v>
+                  <c:v>4023</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2698</c:v>
+                  <c:v>3366</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>434</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>105</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7385</c:v>
+                  <c:v>7189</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>77</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1136</c:v>
+                  <c:v>698</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>466</c:v>
+                  <c:v>1148</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1153</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>485</c:v>
+                  <c:v>1144</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="140274688"/>
-        <c:axId val="82039552"/>
+        <c:axId val="138656768"/>
+        <c:axId val="141947648"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="140274688"/>
+        <c:axId val="138656768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82039552"/>
+        <c:crossAx val="141947648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82039552"/>
+        <c:axId val="141947648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -319,7 +325,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140274688"/>
+        <c:crossAx val="138656768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -353,9 +359,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$16,Tabelle1!$A$18:$A$21)</c:f>
+              <c:f>(Tabelle1!$A$2:$A$16,Tabelle1!$A$17,Tabelle1!$A$18:$A$21)</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>AutoFac       </c:v>
                 </c:pt>
@@ -402,15 +408,18 @@
                   <c:v>SimpleInjector</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>Spring.NET    </c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>StructureMap  </c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>TinyIOC       </c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Unity         </c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Windsor       </c:v>
                 </c:pt>
               </c:strCache>
@@ -418,91 +427,94 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$C$2:$C$16,Tabelle1!$C$18:$C$21)</c:f>
+              <c:f>(Tabelle1!$C$2:$C$16,Tabelle1!$C$17,Tabelle1!$C$18:$C$21)</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2093</c:v>
+                  <c:v>2080</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31564</c:v>
+                  <c:v>1003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>185</c:v>
+                  <c:v>292</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>472</c:v>
+                  <c:v>768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17448</c:v>
+                  <c:v>17818</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9994</c:v>
+                  <c:v>13120</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>693</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19487</c:v>
+                  <c:v>20622</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>85</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>92</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1187</c:v>
+                  <c:v>13792</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2175</c:v>
+                  <c:v>1219</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1872</c:v>
+                  <c:v>1851</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2505</c:v>
+                  <c:v>1723</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="82083840"/>
-        <c:axId val="82085376"/>
+        <c:axId val="141996032"/>
+        <c:axId val="141997568"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="82083840"/>
+        <c:axId val="141996032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82085376"/>
+        <c:crossAx val="141997568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="l"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82085376"/>
+        <c:axId val="141997568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +522,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82083840"/>
+        <c:crossAx val="141996032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -544,9 +556,9 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$16,Tabelle1!$A$18:$A$21)</c:f>
+              <c:f>(Tabelle1!$A$2:$A$16,Tabelle1!$A$17,Tabelle1!$A$18:$A$21)</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>AutoFac       </c:v>
                 </c:pt>
@@ -593,15 +605,18 @@
                   <c:v>SimpleInjector</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>Spring.NET    </c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>StructureMap  </c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>TinyIOC       </c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Unity         </c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Windsor       </c:v>
                 </c:pt>
               </c:strCache>
@@ -609,91 +624,94 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$D$2:$D$16,Tabelle1!$D$18:$D$21)</c:f>
+              <c:f>(Tabelle1!$D$2:$D$16,Tabelle1!$D$17,Tabelle1!$D$18:$D$21)</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5174</c:v>
+                  <c:v>5534</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69224</c:v>
+                  <c:v>3285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>126</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>243</c:v>
+                  <c:v>357</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>458</c:v>
+                  <c:v>679</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2796</c:v>
+                  <c:v>3914</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47403</c:v>
+                  <c:v>57440</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28197</c:v>
+                  <c:v>33682</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1599</c:v>
+                  <c:v>1624</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>395</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54468</c:v>
+                  <c:v>66347</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>244</c:v>
+                  <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>117</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4407</c:v>
+                  <c:v>36551</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7289</c:v>
+                  <c:v>4410</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6202</c:v>
+                  <c:v>6888</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7012</c:v>
+                  <c:v>5792</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="82113280"/>
-        <c:axId val="82114816"/>
+        <c:axId val="142684928"/>
+        <c:axId val="142686464"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="82113280"/>
+        <c:axId val="142684928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82114816"/>
+        <c:crossAx val="142686464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82114816"/>
+        <c:axId val="142686464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +719,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82113280"/>
+        <c:crossAx val="142684928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1099,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B15:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1113,13 +1131,13 @@
         <v>14</v>
       </c>
       <c r="B1" s="2">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C1" s="2">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1127,13 +1145,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="C2" s="2">
-        <v>2093</v>
+        <v>2080</v>
       </c>
       <c r="D2" s="2">
-        <v>5174</v>
+        <v>5534</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1144,13 +1162,13 @@
         <v>20</v>
       </c>
       <c r="B3" s="2">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="C3" s="2">
-        <v>31564</v>
+        <v>1003</v>
       </c>
       <c r="D3" s="2">
-        <v>69224</v>
+        <v>3285</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1161,13 +1179,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>74</v>
-      </c>
-      <c r="C4" s="3">
-        <v>79</v>
+        <v>90</v>
+      </c>
+      <c r="C4" s="4">
+        <v>104</v>
       </c>
       <c r="D4" s="2">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1178,13 +1196,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="D5" s="2">
-        <v>243</v>
+        <v>357</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1195,13 +1213,13 @@
         <v>19</v>
       </c>
       <c r="B6" s="2">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="C6" s="2">
-        <v>185</v>
+        <v>292</v>
       </c>
       <c r="D6" s="2">
-        <v>458</v>
+        <v>679</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1212,13 +1230,13 @@
         <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="C7" s="2">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="D7" s="2">
-        <v>106</v>
+        <v>161</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1229,13 +1247,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>162</v>
+        <v>255</v>
       </c>
       <c r="C8" s="2">
-        <v>472</v>
+        <v>768</v>
       </c>
       <c r="D8" s="2">
-        <v>2796</v>
+        <v>3914</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1246,13 +1264,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>117</v>
-      </c>
-      <c r="C9" s="4">
-        <v>84</v>
+        <v>110</v>
+      </c>
+      <c r="C9" s="3">
+        <v>98</v>
       </c>
       <c r="D9" s="3">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1263,13 +1281,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>2924</v>
+        <v>4023</v>
       </c>
       <c r="C10" s="2">
-        <v>17448</v>
+        <v>17818</v>
       </c>
       <c r="D10" s="2">
-        <v>47403</v>
+        <v>57440</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1280,13 +1298,13 @@
         <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>2698</v>
+        <v>3366</v>
       </c>
       <c r="C11" s="2">
-        <v>9994</v>
+        <v>13120</v>
       </c>
       <c r="D11" s="2">
-        <v>28197</v>
+        <v>33682</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1297,13 +1315,13 @@
         <v>17</v>
       </c>
       <c r="B12" s="2">
-        <v>434</v>
+        <v>365</v>
       </c>
       <c r="C12" s="2">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D12" s="2">
-        <v>1599</v>
+        <v>1624</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1314,13 +1332,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2">
         <v>125</v>
       </c>
       <c r="D13" s="2">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1331,13 +1349,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="2">
-        <v>7385</v>
+        <v>7189</v>
       </c>
       <c r="C14" s="2">
-        <v>19487</v>
+        <v>20622</v>
       </c>
       <c r="D14" s="2">
-        <v>54468</v>
+        <v>66347</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1348,13 +1366,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="2">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C15" s="2">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D15" s="2">
-        <v>244</v>
+        <v>341</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1365,13 +1383,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="3">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D16" s="2">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1382,13 +1400,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="2">
-        <v>811</v>
+        <v>698</v>
       </c>
       <c r="C17" s="2">
-        <v>13566</v>
+        <v>13792</v>
       </c>
       <c r="D17" s="2">
-        <v>37640</v>
+        <v>36551</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1399,13 +1417,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="2">
-        <v>1136</v>
+        <v>1148</v>
       </c>
       <c r="C18" s="2">
-        <v>1187</v>
+        <v>1219</v>
       </c>
       <c r="D18" s="2">
-        <v>4407</v>
+        <v>4410</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1416,13 +1434,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="2">
-        <v>466</v>
+        <v>283</v>
       </c>
       <c r="C19" s="2">
-        <v>2175</v>
+        <v>1851</v>
       </c>
       <c r="D19" s="2">
-        <v>7289</v>
+        <v>6888</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1433,13 +1451,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="2">
-        <v>1153</v>
+        <v>1144</v>
       </c>
       <c r="C20" s="2">
-        <v>1872</v>
+        <v>1723</v>
       </c>
       <c r="D20" s="2">
-        <v>6202</v>
+        <v>5792</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1450,13 +1468,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="2">
-        <v>485</v>
+        <v>501</v>
       </c>
       <c r="C21" s="2">
-        <v>2505</v>
+        <v>2464</v>
       </c>
       <c r="D21" s="2">
-        <v>7012</v>
+        <v>7218</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>

</xml_diff>

<commit_message>
Added performance comparison for interception.
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">AutoFac       </t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Speedioc</t>
+  </si>
+  <si>
+    <t>Singleton</t>
+  </si>
+  <si>
+    <t>Transient</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>Interception</t>
   </si>
 </sst>
 </file>
@@ -168,7 +180,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$23</c:f>
+              <c:f>Tabelle1!$A$3:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
@@ -242,7 +254,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$23</c:f>
+              <c:f>Tabelle1!$B$3:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="22"/>
@@ -317,25 +329,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="129015168"/>
-        <c:axId val="65410176"/>
+        <c:axId val="134454656"/>
+        <c:axId val="144901248"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="129015168"/>
+        <c:axId val="134454656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65410176"/>
+        <c:crossAx val="144901248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65410176"/>
+        <c:axId val="144901248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -343,7 +355,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129015168"/>
+        <c:crossAx val="134454656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -377,7 +389,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$17,Tabelle1!$A$19,Tabelle1!$A$20:$A$23)</c:f>
+              <c:f>(Tabelle1!$A$3:$A$18,Tabelle1!$A$20,Tabelle1!$A$21:$A$24)</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -448,7 +460,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$C$2:$C$17,Tabelle1!$C$19,Tabelle1!$C$20:$C$23)</c:f>
+              <c:f>(Tabelle1!$C$3:$C$18,Tabelle1!$C$20,Tabelle1!$C$21:$C$24)</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="21"/>
@@ -520,25 +532,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="65438080"/>
-        <c:axId val="65439616"/>
+        <c:axId val="144945536"/>
+        <c:axId val="144947072"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="65438080"/>
+        <c:axId val="144945536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65439616"/>
+        <c:crossAx val="144947072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="l"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65439616"/>
+        <c:axId val="144947072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +558,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65438080"/>
+        <c:crossAx val="144945536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -580,7 +592,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Tabelle1!$A$2:$A$17,Tabelle1!$A$19,Tabelle1!$A$20:$A$23)</c:f>
+              <c:f>(Tabelle1!$A$3:$A$18,Tabelle1!$A$20,Tabelle1!$A$21:$A$24)</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -651,7 +663,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$D$2:$D$17,Tabelle1!$D$19,Tabelle1!$D$20:$D$23)</c:f>
+              <c:f>(Tabelle1!$D$3:$D$18,Tabelle1!$D$20,Tabelle1!$D$21:$D$24)</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="21"/>
@@ -723,25 +735,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="65463424"/>
-        <c:axId val="65464960"/>
+        <c:axId val="145626240"/>
+        <c:axId val="145627776"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="65463424"/>
+        <c:axId val="145626240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65464960"/>
+        <c:crossAx val="145627776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65464960"/>
+        <c:axId val="145627776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,7 +761,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65463424"/>
+        <c:crossAx val="145626240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -771,13 +783,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>9523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>8620</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -801,13 +813,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -831,13 +843,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1145,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1157,48 +1169,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="2">
-        <v>39</v>
-      </c>
-      <c r="C1" s="2">
-        <v>52</v>
-      </c>
-      <c r="D1" s="2">
-        <v>82</v>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>974</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2">
-        <v>2310</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
-        <v>6158</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>239</v>
+        <v>974</v>
       </c>
       <c r="C3" s="2">
-        <v>1040</v>
+        <v>2310</v>
       </c>
       <c r="D3" s="2">
-        <v>2830</v>
+        <v>6158</v>
+      </c>
+      <c r="E3">
+        <v>43222</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1206,16 +1221,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <v>239</v>
       </c>
       <c r="C4" s="2">
-        <v>1031</v>
+        <v>1040</v>
       </c>
       <c r="D4" s="2">
-        <v>2863</v>
+        <v>2830</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1223,16 +1238,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
-        <v>79</v>
-      </c>
-      <c r="C5" s="3">
-        <v>87</v>
+        <v>239</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1031</v>
       </c>
       <c r="D5" s="2">
-        <v>142</v>
+        <v>2863</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1240,16 +1255,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2">
-        <v>112</v>
-      </c>
-      <c r="C6" s="2">
-        <v>146</v>
+        <v>79</v>
+      </c>
+      <c r="C6" s="3">
+        <v>87</v>
       </c>
       <c r="D6" s="2">
-        <v>335</v>
+        <v>142</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1257,16 +1272,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>294</v>
+        <v>112</v>
       </c>
       <c r="C7" s="2">
-        <v>257</v>
+        <v>146</v>
       </c>
       <c r="D7" s="2">
-        <v>561</v>
+        <v>335</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1274,16 +1289,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
-        <v>108</v>
+        <v>294</v>
       </c>
       <c r="C8" s="2">
-        <v>107</v>
+        <v>257</v>
       </c>
       <c r="D8" s="2">
-        <v>121</v>
+        <v>561</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1291,16 +1306,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>398</v>
+        <v>108</v>
       </c>
       <c r="C9" s="2">
-        <v>3774</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2">
-        <v>15557</v>
+        <v>121</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1308,16 +1323,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2">
-        <v>96</v>
-      </c>
-      <c r="C10" s="4">
-        <v>92</v>
-      </c>
-      <c r="D10" s="3">
-        <v>103</v>
+        <v>398</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3774</v>
+      </c>
+      <c r="D10" s="2">
+        <v>15557</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1325,16 +1340,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
-        <v>3165</v>
-      </c>
-      <c r="C11" s="2">
-        <v>22788</v>
-      </c>
-      <c r="D11" s="2">
-        <v>52701</v>
+        <v>96</v>
+      </c>
+      <c r="C11" s="4">
+        <v>92</v>
+      </c>
+      <c r="D11" s="3">
+        <v>103</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1342,16 +1357,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>2992</v>
+        <v>3165</v>
       </c>
       <c r="C12" s="2">
-        <v>10728</v>
+        <v>22788</v>
       </c>
       <c r="D12" s="2">
-        <v>31076</v>
+        <v>52701</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1359,16 +1374,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
-        <v>409</v>
+        <v>2992</v>
       </c>
       <c r="C13" s="2">
-        <v>636</v>
+        <v>10728</v>
       </c>
       <c r="D13" s="2">
-        <v>1703</v>
+        <v>31076</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1376,16 +1391,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>115</v>
+        <v>409</v>
       </c>
       <c r="C14" s="2">
-        <v>142</v>
+        <v>636</v>
       </c>
       <c r="D14" s="2">
-        <v>458</v>
+        <v>1703</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1393,16 +1408,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
-        <v>7113</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2">
-        <v>19904</v>
+        <v>142</v>
       </c>
       <c r="D15" s="2">
-        <v>57461</v>
+        <v>458</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1410,16 +1425,16 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2">
-        <v>95</v>
+        <v>7113</v>
       </c>
       <c r="C16" s="2">
-        <v>100</v>
+        <v>19904</v>
       </c>
       <c r="D16" s="2">
-        <v>284</v>
+        <v>57461</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1427,16 +1442,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="4">
-        <v>81</v>
+        <v>7</v>
+      </c>
+      <c r="B17" s="2">
+        <v>95</v>
       </c>
       <c r="C17" s="2">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D17" s="2">
-        <v>134</v>
+        <v>284</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1444,16 +1459,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3">
-        <v>72</v>
+        <v>8</v>
+      </c>
+      <c r="B18" s="4">
+        <v>81</v>
       </c>
       <c r="C18" s="2">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="D18" s="2">
-        <v>123</v>
+        <v>134</v>
+      </c>
+      <c r="E18" s="2">
+        <v>560</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1461,16 +1479,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2">
-        <v>773</v>
+        <v>22</v>
+      </c>
+      <c r="B19" s="3">
+        <v>72</v>
       </c>
       <c r="C19" s="2">
-        <v>14561</v>
+        <v>97</v>
       </c>
       <c r="D19" s="2">
-        <v>38543</v>
+        <v>123</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1478,16 +1496,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2">
-        <v>1238</v>
+        <v>773</v>
       </c>
       <c r="C20" s="2">
-        <v>1249</v>
+        <v>14561</v>
       </c>
       <c r="D20" s="2">
-        <v>4877</v>
+        <v>38543</v>
+      </c>
+      <c r="E20" s="2">
+        <v>897</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1495,16 +1516,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2">
-        <v>264</v>
+        <v>1238</v>
       </c>
       <c r="C21" s="2">
-        <v>1779</v>
+        <v>1249</v>
       </c>
       <c r="D21" s="2">
-        <v>6634</v>
+        <v>4877</v>
+      </c>
+      <c r="E21">
+        <v>11603</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1512,16 +1536,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2">
-        <v>1211</v>
+        <v>264</v>
       </c>
       <c r="C22" s="2">
-        <v>2024</v>
+        <v>1779</v>
       </c>
       <c r="D22" s="2">
-        <v>6346</v>
+        <v>6634</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1529,25 +1553,48 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2">
-        <v>486</v>
+        <v>1211</v>
       </c>
       <c r="C23" s="2">
-        <v>2570</v>
+        <v>2024</v>
       </c>
       <c r="D23" s="2">
-        <v>7585</v>
+        <v>6346</v>
+      </c>
+      <c r="E23">
+        <v>140276</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <v>486</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2570</v>
+      </c>
+      <c r="D24" s="2">
+        <v>7585</v>
+      </c>
+      <c r="E24">
+        <v>26963</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>